<commit_message>
Slightly edited Excel example
</commit_message>
<xml_diff>
--- a/Excel/Dudel_et_al_CFR_Decomposition.xlsx
+++ b/Excel/Dudel_et_al_CFR_Decomposition.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="69">
   <si>
     <t>Age group</t>
   </si>
@@ -662,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G128"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,1104 +684,1115 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="15">
-        <f>G41</f>
-        <v>1.4175954983226923E-2</v>
-      </c>
-      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="15">
-        <f>G57</f>
-        <v>7.5836338375560031E-2</v>
+        <f>G43</f>
+        <v>1.4175954983226923E-2</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="15">
-        <f>B7-B9</f>
-        <v>-6.166038339233311E-2</v>
+        <f>G59</f>
+        <v>7.5836338375560031E-2</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="15">
-        <f>D121</f>
-        <v>0.56427055420919481</v>
+        <f>B9-B11</f>
+        <v>-6.166038339233311E-2</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="15">
+        <f>D123</f>
+        <v>0.56427055420919481</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="15">
-        <f>D125</f>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
+        <f>D127</f>
         <v>0.43572944579080514</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+    <row r="20" spans="1:7" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="26" spans="1:7" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="28" spans="1:7" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" t="str">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="str">
         <f>"0-9"</f>
         <v>0-9</v>
       </c>
-      <c r="D32">
+      <c r="D34">
         <v>106</v>
       </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32" s="5">
-        <f>D32/SUM($D$32:$D$40)</f>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <f t="shared" ref="F34:F42" si="0">D34/SUM($D$34:$D$42)</f>
         <v>1.1470620062763771E-2</v>
       </c>
-      <c r="G32" s="5">
-        <f>E32/D32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="str">
+      <c r="G34" s="5">
+        <f>E34/D34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="str">
         <f>"10-19"</f>
         <v>10-19</v>
       </c>
-      <c r="D33">
+      <c r="D35">
         <v>488</v>
       </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33" s="5">
-        <f>D33/SUM($D$32:$D$40)</f>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="5">
+        <f t="shared" si="0"/>
         <v>5.2808137647440752E-2</v>
       </c>
-      <c r="G33" s="5">
-        <f t="shared" ref="G33:G40" si="0">E33/D33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" t="str">
+      <c r="G35" s="5">
+        <f t="shared" ref="G35:G42" si="1">E35/D35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="str">
         <f>"20-29"</f>
         <v>20-29</v>
       </c>
-      <c r="D34">
+      <c r="D36">
         <v>2508</v>
       </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34" s="5">
-        <f>D34/SUM($D$32:$D$40)</f>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <f t="shared" si="0"/>
         <v>0.27139919922086353</v>
       </c>
-      <c r="G34" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" t="str">
+      <c r="G36" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="str">
         <f>"30-39"</f>
         <v>30-39</v>
       </c>
-      <c r="D35">
+      <c r="D37">
         <v>955</v>
       </c>
-      <c r="E35">
+      <c r="E37">
         <v>1</v>
       </c>
-      <c r="F35" s="5">
-        <f>D35/SUM($D$32:$D$40)</f>
+      <c r="F37" s="5">
+        <f t="shared" si="0"/>
         <v>0.10334379396169245</v>
       </c>
-      <c r="G35" s="5">
-        <f t="shared" si="0"/>
+      <c r="G37" s="5">
+        <f t="shared" si="1"/>
         <v>1.0471204188481676E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" t="str">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="str">
         <f>"40-49"</f>
         <v>40-49</v>
       </c>
-      <c r="D36">
+      <c r="D38">
         <v>1252</v>
       </c>
-      <c r="E36">
+      <c r="E38">
         <v>1</v>
       </c>
-      <c r="F36" s="5">
-        <f>D36/SUM($D$32:$D$40)</f>
+      <c r="F38" s="5">
+        <f t="shared" si="0"/>
         <v>0.13548317281679473</v>
       </c>
-      <c r="G36" s="5">
-        <f t="shared" si="0"/>
+      <c r="G38" s="5">
+        <f t="shared" si="1"/>
         <v>7.9872204472843447E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" t="str">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="str">
         <f>"50-59"</f>
         <v>50-59</v>
       </c>
-      <c r="D37">
+      <c r="D39">
         <v>1738</v>
       </c>
-      <c r="E37">
+      <c r="E39">
         <v>10</v>
       </c>
-      <c r="F37" s="5">
-        <f>D37/SUM($D$32:$D$40)</f>
+      <c r="F39" s="5">
+        <f t="shared" si="0"/>
         <v>0.18807488367059841</v>
       </c>
-      <c r="G37" s="5">
-        <f t="shared" si="0"/>
+      <c r="G39" s="5">
+        <f t="shared" si="1"/>
         <v>5.7537399309551211E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="str">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="str">
         <f>"60-69"</f>
         <v>60-69</v>
       </c>
-      <c r="D38">
+      <c r="D40">
         <v>1162</v>
       </c>
-      <c r="E38">
+      <c r="E40">
         <v>20</v>
       </c>
-      <c r="F38" s="5">
-        <f>D38/SUM($D$32:$D$40)</f>
+      <c r="F40" s="5">
+        <f t="shared" si="0"/>
         <v>0.12574396710312738</v>
       </c>
-      <c r="G38" s="5">
-        <f t="shared" si="0"/>
+      <c r="G40" s="5">
+        <f t="shared" si="1"/>
         <v>1.7211703958691909E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" t="str">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="str">
         <f>"70-79"</f>
         <v>70-79</v>
       </c>
-      <c r="D39">
+      <c r="D41">
         <v>616</v>
       </c>
-      <c r="E39">
+      <c r="E41">
         <v>41</v>
       </c>
-      <c r="F39" s="5">
-        <f>D39/SUM($D$32:$D$40)</f>
+      <c r="F41" s="5">
+        <f t="shared" si="0"/>
         <v>6.6659452440212097E-2</v>
       </c>
-      <c r="G39" s="5">
-        <f t="shared" si="0"/>
+      <c r="G41" s="5">
+        <f t="shared" si="1"/>
         <v>6.6558441558441553E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" t="str">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="str">
         <f>"80+"</f>
         <v>80+</v>
       </c>
-      <c r="D40">
+      <c r="D42">
         <v>416</v>
       </c>
-      <c r="E40">
+      <c r="E42">
         <v>58</v>
       </c>
-      <c r="F40" s="5">
-        <f>D40/SUM($D$32:$D$40)</f>
+      <c r="F42" s="5">
+        <f t="shared" si="0"/>
         <v>4.5016773076506873E-2</v>
       </c>
-      <c r="G40" s="5">
-        <f t="shared" si="0"/>
+      <c r="G42" s="5">
+        <f t="shared" si="1"/>
         <v>0.13942307692307693</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8">
-        <f>SUM(D32:D40)</f>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8">
+        <f>SUM(D34:D42)</f>
         <v>9241</v>
       </c>
-      <c r="E41" s="8">
-        <f>SUM(E32:E40)</f>
+      <c r="E43" s="8">
+        <f>SUM(E34:E42)</f>
         <v>131</v>
       </c>
-      <c r="F41" s="10">
-        <f>SUM(F32:F40)</f>
+      <c r="F43" s="10">
+        <f>SUM(F34:F42)</f>
         <v>1</v>
       </c>
-      <c r="G41" s="10">
-        <f>E41/D41</f>
+      <c r="G43" s="10">
+        <f>E43/D43</f>
         <v>1.4175954983226923E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" t="str">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="str">
         <f>"0-9"</f>
         <v>0-9</v>
       </c>
-      <c r="D47">
+      <c r="D49">
         <v>181</v>
       </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47" s="5">
-        <f>D47/($D$57-$D$56)</f>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" s="5">
+        <f>D49/($D$59-$D$58)</f>
         <v>5.2848258343309289E-3</v>
       </c>
-      <c r="G47" s="5">
-        <f>(E47+$E$56*E47/SUM($E$47:$E$55))/(D47+F47*$D$56)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="str">
+      <c r="G49" s="5">
+        <f>(E49+$E$58*E49/SUM($E$49:$E$57))/(D49+F49*$D$58)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="str">
         <f>"10-19"</f>
         <v>10-19</v>
       </c>
-      <c r="D48">
+      <c r="D50">
         <v>312</v>
       </c>
-      <c r="E48">
+      <c r="E50">
         <v>1</v>
       </c>
-      <c r="F48" s="5">
-        <f t="shared" ref="F48:F55" si="1">D48/($D$57-$D$56)</f>
+      <c r="F50" s="5">
+        <f t="shared" ref="F50:F57" si="2">D50/($D$59-$D$58)</f>
         <v>9.109755029343922E-3</v>
       </c>
-      <c r="G48" s="5">
-        <f t="shared" ref="G48:G55" si="2">(E48+$E$56*E48/SUM($E$47:$E$55))/(D48+F48*$D$56)</f>
+      <c r="G50" s="5">
+        <f t="shared" ref="G50:G57" si="3">(E50+$E$58*E50/SUM($E$49:$E$57))/(D50+F50*$D$58)</f>
         <v>6.0897875589081361E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B49" t="str">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="str">
         <f>"20-29"</f>
         <v>20-29</v>
       </c>
-      <c r="D49">
+      <c r="D51">
         <v>2011</v>
       </c>
-      <c r="E49">
+      <c r="E51">
         <v>4</v>
       </c>
-      <c r="F49" s="5">
-        <f t="shared" si="1"/>
+      <c r="F51" s="5">
+        <f t="shared" si="2"/>
         <v>5.87170428333674E-2</v>
       </c>
-      <c r="G49" s="5">
-        <f t="shared" si="2"/>
+      <c r="G51" s="5">
+        <f t="shared" si="3"/>
         <v>3.7792416079151432E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B50" t="str">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="str">
         <f>"30-39"</f>
         <v>30-39</v>
       </c>
-      <c r="D50">
+      <c r="D52">
         <v>3575</v>
       </c>
-      <c r="E50">
+      <c r="E52">
         <v>7</v>
       </c>
-      <c r="F50" s="5">
-        <f t="shared" si="1"/>
+      <c r="F52" s="5">
+        <f t="shared" si="2"/>
         <v>0.10438260971123245</v>
       </c>
-      <c r="G50" s="5">
-        <f t="shared" si="2"/>
+      <c r="G52" s="5">
+        <f t="shared" si="3"/>
         <v>3.7203065814420612E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B51" t="str">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="str">
         <f>"40-49"</f>
         <v>40-49</v>
       </c>
-      <c r="D51">
+      <c r="D53">
         <v>5242</v>
       </c>
-      <c r="E51">
+      <c r="E53">
         <v>19</v>
       </c>
-      <c r="F51" s="5">
-        <f t="shared" si="1"/>
+      <c r="F53" s="5">
+        <f t="shared" si="2"/>
         <v>0.15305556366609244</v>
       </c>
-      <c r="G51" s="5">
-        <f t="shared" si="2"/>
+      <c r="G53" s="5">
+        <f t="shared" si="3"/>
         <v>6.8867341948125587E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B52" t="str">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="str">
         <f>"50-59"</f>
         <v>50-59</v>
       </c>
-      <c r="D52">
+      <c r="D54">
         <v>6030</v>
       </c>
-      <c r="E52">
+      <c r="E54">
         <v>35</v>
       </c>
-      <c r="F52" s="5">
-        <f t="shared" si="1"/>
+      <c r="F54" s="5">
+        <f t="shared" si="2"/>
         <v>0.17606353470174313</v>
       </c>
-      <c r="G52" s="5">
-        <f t="shared" si="2"/>
+      <c r="G54" s="5">
+        <f t="shared" si="3"/>
         <v>1.1028271997226674E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B53" t="str">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="str">
         <f>"60-69"</f>
         <v>60-69</v>
       </c>
-      <c r="D53">
+      <c r="D55">
         <v>5633</v>
       </c>
-      <c r="E53">
+      <c r="E55">
         <v>119</v>
       </c>
-      <c r="F53" s="5">
-        <f t="shared" si="1"/>
+      <c r="F55" s="5">
+        <f t="shared" si="2"/>
         <v>0.1644719553855587</v>
       </c>
-      <c r="G53" s="5">
-        <f t="shared" si="2"/>
+      <c r="G55" s="5">
+        <f t="shared" si="3"/>
         <v>4.0138759539701981E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B54" t="str">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="str">
         <f>"70-79"</f>
         <v>70-79</v>
       </c>
-      <c r="D54">
+      <c r="D56">
         <v>5620</v>
       </c>
-      <c r="E54">
+      <c r="E56">
         <v>319</v>
       </c>
-      <c r="F54" s="5">
-        <f t="shared" si="1"/>
+      <c r="F56" s="5">
+        <f t="shared" si="2"/>
         <v>0.16409238225933603</v>
       </c>
-      <c r="G54" s="5">
-        <f t="shared" si="2"/>
+      <c r="G56" s="5">
+        <f t="shared" si="3"/>
         <v>0.10784775376565997</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B55" t="str">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="str">
         <f>"80+"</f>
         <v>80+</v>
       </c>
-      <c r="D55">
+      <c r="D57">
         <v>5645</v>
       </c>
-      <c r="E55">
+      <c r="E57">
         <v>863</v>
       </c>
-      <c r="F55" s="5">
-        <f t="shared" si="1"/>
+      <c r="F57" s="5">
+        <f t="shared" si="2"/>
         <v>0.16482233057899501</v>
       </c>
-      <c r="G55" s="5">
-        <f t="shared" si="2"/>
+      <c r="G57" s="5">
+        <f t="shared" si="3"/>
         <v>0.29047153923142055</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>41</v>
       </c>
-      <c r="D56">
+      <c r="D58">
         <v>29810</v>
       </c>
-      <c r="E56">
+      <c r="E58">
         <v>3491</v>
       </c>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8">
-        <f>SUM(D47:D56)</f>
-        <v>64059</v>
-      </c>
-      <c r="E57" s="8">
-        <f>SUM(E47:E56)</f>
-        <v>4858</v>
-      </c>
-      <c r="F57" s="10">
-        <f>SUM(F47:F56)</f>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="G57" s="10">
-        <f>E57/D57</f>
-        <v>7.5836338375560031E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="60" spans="1:7" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="9" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8">
+        <f>SUM(D49:D58)</f>
+        <v>64059</v>
+      </c>
+      <c r="E59" s="8">
+        <f>SUM(E49:E58)</f>
+        <v>4858</v>
+      </c>
+      <c r="F59" s="10">
+        <f>SUM(F49:F58)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="G59" s="10">
+        <f>E59/D59</f>
+        <v>7.5836338375560031E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="62" spans="1:7" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6" t="s">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="E66" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" t="str">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" t="str">
         <f>"0-9"</f>
         <v>0-9</v>
       </c>
-      <c r="D66" s="5">
-        <f>F32*G47</f>
-        <v>0</v>
-      </c>
-      <c r="E66" s="5">
-        <f>F47*G32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="str">
+      <c r="D68" s="5">
+        <f t="shared" ref="D68:D76" si="4">F34*G49</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="5">
+        <f t="shared" ref="E68:E76" si="5">F49*G34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="str">
         <f>"10-19"</f>
         <v>10-19</v>
       </c>
-      <c r="D67" s="5">
-        <f>F33*G48</f>
+      <c r="D69" s="5">
+        <f t="shared" si="4"/>
         <v>3.2159033965449308E-4</v>
       </c>
-      <c r="E67" s="5">
-        <f>F48*G33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" t="str">
+      <c r="E69" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" t="str">
         <f>"20-29"</f>
         <v>20-29</v>
       </c>
-      <c r="D68" s="5">
-        <f>F34*G49</f>
+      <c r="D70" s="5">
+        <f t="shared" si="4"/>
         <v>1.0256831460503386E-3</v>
       </c>
-      <c r="E68" s="5">
-        <f>F49*G34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" t="str">
+      <c r="E70" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" t="str">
         <f>"30-39"</f>
         <v>30-39</v>
       </c>
-      <c r="D69" s="5">
-        <f>F35*G50</f>
+      <c r="D71" s="5">
+        <f t="shared" si="4"/>
         <v>3.8447059682687675E-4</v>
       </c>
-      <c r="E69" s="5">
-        <f>F50*G35</f>
+      <c r="E71" s="5">
+        <f t="shared" si="5"/>
         <v>1.0930116200129053E-4</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" t="str">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" t="str">
         <f>"40-49"</f>
         <v>40-49</v>
       </c>
-      <c r="D70" s="5">
-        <f>F36*G51</f>
+      <c r="D72" s="5">
+        <f t="shared" si="4"/>
         <v>9.3303659905911963E-4</v>
       </c>
-      <c r="E70" s="5">
-        <f>F51*G36</f>
+      <c r="E72" s="5">
+        <f t="shared" si="5"/>
         <v>1.2224885276844444E-4</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" t="str">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" t="str">
         <f>"50-59"</f>
         <v>50-59</v>
       </c>
-      <c r="D71" s="5">
-        <f>F37*G52</f>
+      <c r="D73" s="5">
+        <f t="shared" si="4"/>
         <v>2.0741409729661247E-3</v>
       </c>
-      <c r="E71" s="5">
-        <f>F52*G37</f>
+      <c r="E73" s="5">
+        <f t="shared" si="5"/>
         <v>1.0130237899985222E-3</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" t="str">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" t="str">
         <f>"60-69"</f>
         <v>60-69</v>
       </c>
-      <c r="D72" s="5">
-        <f>F38*G53</f>
+      <c r="D74" s="5">
+        <f t="shared" si="4"/>
         <v>5.0472068591206265E-3</v>
       </c>
-      <c r="E72" s="5">
-        <f>F53*G38</f>
+      <c r="E74" s="5">
+        <f t="shared" si="5"/>
         <v>2.8308426056034195E-3</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" t="str">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" t="str">
         <f>"70-79"</f>
         <v>70-79</v>
       </c>
-      <c r="D73" s="5">
-        <f>F39*G54</f>
+      <c r="D75" s="5">
+        <f t="shared" si="4"/>
         <v>7.1890722129257156E-3</v>
       </c>
-      <c r="E73" s="5">
-        <f>F54*G39</f>
+      <c r="E75" s="5">
+        <f t="shared" si="5"/>
         <v>1.0921733234793469E-2</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" t="str">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" t="str">
         <f>"80+"</f>
         <v>80+</v>
       </c>
-      <c r="D74" s="5">
-        <f>F40*G55</f>
+      <c r="D76" s="5">
+        <f t="shared" si="4"/>
         <v>1.3076091366764523E-2</v>
       </c>
-      <c r="E74" s="5">
-        <f>F55*G40</f>
+      <c r="E76" s="5">
+        <f t="shared" si="5"/>
         <v>2.2980036474956035E-2</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="8" t="s">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="10">
-        <f>SUM(D66:D74)</f>
+      <c r="C77" s="8"/>
+      <c r="D77" s="10">
+        <f>SUM(D68:D76)</f>
         <v>3.0051292093367817E-2</v>
       </c>
-      <c r="E75" s="10">
-        <f>SUM(E66:E74)</f>
+      <c r="E77" s="10">
+        <f>SUM(E68:E76)</f>
         <v>3.797718612012118E-2</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>40</v>
-      </c>
-      <c r="D81" s="5">
-        <f>G57</f>
-        <v>7.5836338375560031E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>34</v>
-      </c>
-      <c r="D82" s="5">
-        <f>D75</f>
-        <v>3.0051292093367817E-2</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D83" s="5">
-        <f>E75</f>
-        <v>3.797718612012118E-2</v>
+        <f>G59</f>
+        <v>7.5836338375560031E-2</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
+        <v>34</v>
+      </c>
+      <c r="D84" s="5">
+        <f>D77</f>
+        <v>3.0051292093367817E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="D85" s="5">
+        <f>E77</f>
+        <v>3.797718612012118E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>15</v>
       </c>
-      <c r="D84" s="5">
-        <f>G41</f>
+      <c r="D86" s="5">
+        <f>G43</f>
         <v>1.4175954983226923E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="1" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D86" s="5">
-        <f>0.5*(D84-D83+D82-D81)</f>
+      <c r="D88" s="5">
+        <f>0.5*(D86-D85+D84-D83)</f>
         <v>-3.4793138709543238E-2</v>
       </c>
-      <c r="F86" t="str">
+      <c r="F88" t="str">
         <f>"Formula = 0.5*(CFR SK- Hyp.1 SK + Hyp.1 ES - CFR ES)"</f>
         <v>Formula = 0.5*(CFR SK- Hyp.1 SK + Hyp.1 ES - CFR ES)</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="1"/>
-      <c r="D87" s="5"/>
-    </row>
-    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="12" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B89" s="1"/>
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B90" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6" t="s">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E90" s="6" t="s">
+      <c r="E92" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B92" t="str">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B94" t="str">
         <f>"0-9"</f>
         <v>0-9</v>
       </c>
-      <c r="D92" s="5">
-        <f>F47*G32</f>
-        <v>0</v>
-      </c>
-      <c r="E92" s="5">
-        <f>F32*G47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="str">
+      <c r="D94" s="5">
+        <f t="shared" ref="D94:D102" si="6">F49*G34</f>
+        <v>0</v>
+      </c>
+      <c r="E94" s="5">
+        <f t="shared" ref="E94:E102" si="7">F34*G49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="str">
         <f>"10-19"</f>
         <v>10-19</v>
       </c>
-      <c r="D93" s="5">
-        <f>F48*G33</f>
-        <v>0</v>
-      </c>
-      <c r="E93" s="5">
-        <f>F33*G48</f>
+      <c r="D95" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E95" s="5">
+        <f t="shared" si="7"/>
         <v>3.2159033965449308E-4</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B94" t="str">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B96" t="str">
         <f>"20-29"</f>
         <v>20-29</v>
       </c>
-      <c r="D94" s="5">
-        <f>F49*G34</f>
-        <v>0</v>
-      </c>
-      <c r="E94" s="5">
-        <f>F34*G49</f>
+      <c r="D96" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E96" s="5">
+        <f t="shared" si="7"/>
         <v>1.0256831460503386E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B95" t="str">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" t="str">
         <f>"30-39"</f>
         <v>30-39</v>
       </c>
-      <c r="D95" s="5">
-        <f>F50*G35</f>
+      <c r="D97" s="5">
+        <f t="shared" si="6"/>
         <v>1.0930116200129053E-4</v>
       </c>
-      <c r="E95" s="5">
-        <f>F35*G50</f>
+      <c r="E97" s="5">
+        <f t="shared" si="7"/>
         <v>3.8447059682687675E-4</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B96" t="str">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" t="str">
         <f>"40-49"</f>
         <v>40-49</v>
       </c>
-      <c r="D96" s="5">
-        <f>F51*G36</f>
+      <c r="D98" s="5">
+        <f t="shared" si="6"/>
         <v>1.2224885276844444E-4</v>
       </c>
-      <c r="E96" s="5">
-        <f>F36*G51</f>
+      <c r="E98" s="5">
+        <f t="shared" si="7"/>
         <v>9.3303659905911963E-4</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" t="str">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" t="str">
         <f>"50-59"</f>
         <v>50-59</v>
       </c>
-      <c r="D97" s="5">
-        <f>F52*G37</f>
+      <c r="D99" s="5">
+        <f t="shared" si="6"/>
         <v>1.0130237899985222E-3</v>
       </c>
-      <c r="E97" s="5">
-        <f>F37*G52</f>
+      <c r="E99" s="5">
+        <f t="shared" si="7"/>
         <v>2.0741409729661247E-3</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B98" t="str">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" t="str">
         <f>"60-69"</f>
         <v>60-69</v>
       </c>
-      <c r="D98" s="5">
-        <f>F53*G38</f>
+      <c r="D100" s="5">
+        <f t="shared" si="6"/>
         <v>2.8308426056034195E-3</v>
       </c>
-      <c r="E98" s="5">
-        <f>F38*G53</f>
+      <c r="E100" s="5">
+        <f t="shared" si="7"/>
         <v>5.0472068591206265E-3</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B99" t="str">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" t="str">
         <f>"70-79"</f>
         <v>70-79</v>
       </c>
-      <c r="D99" s="5">
-        <f>F54*G39</f>
+      <c r="D101" s="5">
+        <f t="shared" si="6"/>
         <v>1.0921733234793469E-2</v>
       </c>
-      <c r="E99" s="5">
-        <f>F39*G54</f>
+      <c r="E101" s="5">
+        <f t="shared" si="7"/>
         <v>7.1890722129257156E-3</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B100" t="str">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" t="str">
         <f>"80+"</f>
         <v>80+</v>
       </c>
-      <c r="D100" s="5">
-        <f>F55*G40</f>
+      <c r="D102" s="5">
+        <f t="shared" si="6"/>
         <v>2.2980036474956035E-2</v>
       </c>
-      <c r="E100" s="5">
-        <f>F40*G55</f>
+      <c r="E102" s="5">
+        <f t="shared" si="7"/>
         <v>1.3076091366764523E-2</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B101" s="8" t="s">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C101" s="8"/>
-      <c r="D101" s="10">
-        <f>SUM(D92:D100)</f>
+      <c r="C103" s="8"/>
+      <c r="D103" s="10">
+        <f>SUM(D94:D102)</f>
         <v>3.797718612012118E-2</v>
       </c>
-      <c r="E101" s="10">
-        <f>SUM(E92:E100)</f>
+      <c r="E103" s="10">
+        <f>SUM(E94:E102)</f>
         <v>3.0051292093367817E-2</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
         <v>40</v>
       </c>
-      <c r="D107" s="5">
-        <f>G57</f>
+      <c r="D109" s="5">
+        <f>G59</f>
         <v>7.5836338375560031E-2</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
         <v>37</v>
       </c>
-      <c r="D108" s="5">
-        <f>D101</f>
+      <c r="D110" s="5">
+        <f>D103</f>
         <v>3.797718612012118E-2</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
         <v>22</v>
       </c>
-      <c r="D109" s="5">
-        <f>E101</f>
+      <c r="D111" s="5">
+        <f>E103</f>
         <v>3.0051292093367817E-2</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
         <v>15</v>
       </c>
-      <c r="D110" s="5">
-        <f>G41</f>
+      <c r="D112" s="5">
+        <f>G43</f>
         <v>1.4175954983226923E-2</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B112" s="1" t="s">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B114" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D112" s="5">
-        <f>0.5*(D110-D109+D108-D107)</f>
+      <c r="D114" s="5">
+        <f>0.5*(D112-D111+D110-D109)</f>
         <v>-2.6867244682789872E-2</v>
       </c>
-      <c r="F112" t="str">
+      <c r="F114" t="str">
         <f>"Formula = 0.5*(CFR SK - Hyp.2 SK + Hyp.2 ES - CFR ES)"</f>
         <v>Formula = 0.5*(CFR SK - Hyp.2 SK + Hyp.2 ES - CFR ES)</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="12" t="s">
+    <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="2" t="s">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B118" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="5">
-        <f>G41-G57</f>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B119" s="5">
+        <f>G43-G59</f>
         <v>-6.166038339233311E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="2" t="s">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="1" t="s">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B122" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="5">
-        <f>D86</f>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B123" s="5">
+        <f>D88</f>
         <v>-3.4793138709543238E-2</v>
       </c>
-      <c r="D121" s="15">
-        <f>ABS(B121)/(ABS(B121)+ABS(B125))</f>
+      <c r="D123" s="15">
+        <f>ABS(B123)/(ABS(B123)+ABS(B127))</f>
         <v>0.56427055420919481</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="2" t="s">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B125" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="1" t="s">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B126" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="5">
-        <f>D112</f>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B127" s="5">
+        <f>D114</f>
         <v>-2.6867244682789872E-2</v>
       </c>
-      <c r="D125" s="15">
-        <f>ABS(B125)/(ABS(B121)+ABS(B125))</f>
+      <c r="D127" s="15">
+        <f>ABS(B127)/(ABS(B123)+ABS(B127))</f>
         <v>0.43572944579080514</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="5"/>
-    </row>
-    <row r="128" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="5"/>
+    </row>
+    <row r="130" spans="2:2" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1793,7 +1804,7 @@
   <dimension ref="A1:G130"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,11 +2449,11 @@
         <v>0-9</v>
       </c>
       <c r="D68" s="5">
-        <f>F50*G35</f>
+        <f t="shared" ref="D68:D76" si="4">F50*G35</f>
         <v>0</v>
       </c>
       <c r="E68" s="5">
-        <f>F35*G50</f>
+        <f t="shared" ref="E68:E76" si="5">F35*G50</f>
         <v>0</v>
       </c>
     </row>
@@ -2452,11 +2463,11 @@
         <v>10-19</v>
       </c>
       <c r="D69" s="5">
-        <f>F51*G36</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E69" s="5">
-        <f>F36*G51</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2466,11 +2477,11 @@
         <v>20-29</v>
       </c>
       <c r="D70" s="5">
-        <f>F52*G37</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E70" s="5">
-        <f>F37*G52</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2480,11 +2491,11 @@
         <v>30-39</v>
       </c>
       <c r="D71" s="5">
-        <f>F53*G38</f>
+        <f t="shared" si="4"/>
         <v>2.4554800807784102E-4</v>
       </c>
       <c r="E71" s="5">
-        <f>F38*G53</f>
+        <f t="shared" si="5"/>
         <v>7.8698658516565968E-5</v>
       </c>
     </row>
@@ -2494,11 +2505,11 @@
         <v>40-49</v>
       </c>
       <c r="D72" s="5">
-        <f>F54*G39</f>
+        <f t="shared" si="4"/>
         <v>4.2041222550404523E-4</v>
       </c>
       <c r="E72" s="5">
-        <f>F39*G54</f>
+        <f t="shared" si="5"/>
         <v>1.0342152236757176E-4</v>
       </c>
     </row>
@@ -2508,11 +2519,11 @@
         <v>50-59</v>
       </c>
       <c r="D73" s="5">
-        <f>F55*G40</f>
+        <f t="shared" si="4"/>
         <v>1.870978356244516E-3</v>
       </c>
       <c r="E73" s="5">
-        <f>F40*G55</f>
+        <f t="shared" si="5"/>
         <v>7.126627709575017E-4</v>
       </c>
     </row>
@@ -2522,11 +2533,11 @@
         <v>60-69</v>
       </c>
       <c r="D74" s="5">
-        <f>F56*G41</f>
+        <f t="shared" si="4"/>
         <v>4.0285818282663711E-3</v>
       </c>
       <c r="E74" s="5">
-        <f>F41*G56</f>
+        <f t="shared" si="5"/>
         <v>2.7629564458873496E-3</v>
       </c>
     </row>
@@ -2536,11 +2547,11 @@
         <v>70-79</v>
       </c>
       <c r="D75" s="5">
-        <f>F57*G42</f>
+        <f t="shared" si="4"/>
         <v>7.612679995195124E-3</v>
       </c>
       <c r="E75" s="5">
-        <f>F42*G57</f>
+        <f t="shared" si="5"/>
         <v>1.1079002707053904E-2</v>
       </c>
     </row>
@@ -2550,11 +2561,11 @@
         <v>80+</v>
       </c>
       <c r="D76" s="5">
-        <f>F58*G43</f>
+        <f t="shared" si="4"/>
         <v>6.3364886838786754E-3</v>
       </c>
       <c r="E76" s="5">
-        <f>F43*G58</f>
+        <f t="shared" si="5"/>
         <v>1.9042237421822348E-2</v>
       </c>
     </row>
@@ -2658,11 +2669,11 @@
         <v>0-9</v>
       </c>
       <c r="D94" s="5">
-        <f>F35*G50</f>
+        <f t="shared" ref="D94:D102" si="6">F35*G50</f>
         <v>0</v>
       </c>
       <c r="E94" s="5">
-        <f>F50*G35</f>
+        <f t="shared" ref="E94:E102" si="7">F50*G35</f>
         <v>0</v>
       </c>
     </row>
@@ -2672,11 +2683,11 @@
         <v>10-19</v>
       </c>
       <c r="D95" s="5">
-        <f>F36*G51</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E95" s="5">
-        <f>F51*G36</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2686,11 +2697,11 @@
         <v>20-29</v>
       </c>
       <c r="D96" s="5">
-        <f>F37*G52</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E96" s="5">
-        <f>F52*G37</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2700,11 +2711,11 @@
         <v>30-39</v>
       </c>
       <c r="D97" s="5">
-        <f>F38*G53</f>
+        <f t="shared" si="6"/>
         <v>7.8698658516565968E-5</v>
       </c>
       <c r="E97" s="5">
-        <f>F53*G38</f>
+        <f t="shared" si="7"/>
         <v>2.4554800807784102E-4</v>
       </c>
     </row>
@@ -2714,11 +2725,11 @@
         <v>40-49</v>
       </c>
       <c r="D98" s="5">
-        <f>F39*G54</f>
+        <f t="shared" si="6"/>
         <v>1.0342152236757176E-4</v>
       </c>
       <c r="E98" s="5">
-        <f>F54*G39</f>
+        <f t="shared" si="7"/>
         <v>4.2041222550404523E-4</v>
       </c>
     </row>
@@ -2728,11 +2739,11 @@
         <v>50-59</v>
       </c>
       <c r="D99" s="5">
-        <f>F40*G55</f>
+        <f t="shared" si="6"/>
         <v>7.126627709575017E-4</v>
       </c>
       <c r="E99" s="5">
-        <f>F55*G40</f>
+        <f t="shared" si="7"/>
         <v>1.870978356244516E-3</v>
       </c>
     </row>
@@ -2742,11 +2753,11 @@
         <v>60-69</v>
       </c>
       <c r="D100" s="5">
-        <f>F41*G56</f>
+        <f t="shared" si="6"/>
         <v>2.7629564458873496E-3</v>
       </c>
       <c r="E100" s="5">
-        <f>F56*G41</f>
+        <f t="shared" si="7"/>
         <v>4.0285818282663711E-3</v>
       </c>
     </row>
@@ -2756,11 +2767,11 @@
         <v>70-79</v>
       </c>
       <c r="D101" s="5">
-        <f>F42*G57</f>
+        <f t="shared" si="6"/>
         <v>1.1079002707053904E-2</v>
       </c>
       <c r="E101" s="5">
-        <f>F57*G42</f>
+        <f t="shared" si="7"/>
         <v>7.612679995195124E-3</v>
       </c>
     </row>
@@ -2770,11 +2781,11 @@
         <v>80+</v>
       </c>
       <c r="D102" s="5">
-        <f>F43*G58</f>
+        <f t="shared" si="6"/>
         <v>1.9042237421822348E-2</v>
       </c>
       <c r="E102" s="5">
-        <f>F58*G43</f>
+        <f t="shared" si="7"/>
         <v>6.3364886838786754E-3</v>
       </c>
     </row>

</xml_diff>